<commit_message>
found mistake in acceptance test
</commit_message>
<xml_diff>
--- a/etc/2185-swen-261-04-d damns.xlsx
+++ b/etc/2185-swen-261-04-d damns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suwamik Paul\Desktop\SWEN\team-project-2185-swen-261-04-d-damns\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AB78AD4-B16E-4482-9B56-F51E215401E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92E12C6-0EA7-463E-B111-C072E3E05541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>Instructions</t>
   </si>
@@ -306,14 +306,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <fill>
         <patternFill>
@@ -479,13 +472,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -902,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -950,9 +936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H599"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1351,9 +1337,6 @@
       </c>
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
@@ -1362,9 +1345,6 @@
       </c>
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -4225,138 +4205,138 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D599">
-    <cfRule type="expression" dxfId="33" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F18 F30 F33:F599">
-    <cfRule type="expression" dxfId="31" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H599">
-    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
       <formula>AND(ISBLANK(F19),E19="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
       <formula>AND(ISBLANK(F19),E19="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>AND(ISBLANK(F20),E20="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>AND(ISBLANK(F20),E20="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
       <formula>AND(ISBLANK(F21),E21="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
       <formula>AND(ISBLANK(F21),E21="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>AND(ISBLANK(F22),E22="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>AND(ISBLANK(F22),E22="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>AND(ISBLANK(F23),E23="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
       <formula>AND(ISBLANK(F23),E23="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>AND(ISBLANK(F24),E24="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>AND(ISBLANK(F24),E24="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>AND(ISBLANK(F25),E25="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>AND(ISBLANK(F25),E25="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>AND(ISBLANK(F26),E26="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>AND(ISBLANK(F26),E26="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>AND(ISBLANK(F27),E27="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>AND(ISBLANK(F27),E27="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>AND(ISBLANK(F28),E28="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
       <formula>AND(ISBLANK(F28),E28="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(F29),E29="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(F29),E29="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(F31),E31="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(F31),E31="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(ISBLANK(F32),E32="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND(ISBLANK(F32),E32="Fail")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>